<commit_message>
more data tidying and validating
</commit_message>
<xml_diff>
--- a/docs/MM-for-calculator.xlsx
+++ b/docs/MM-for-calculator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="7600" windowWidth="35880" windowHeight="19500" tabRatio="500"/>
+    <workbookView xWindow="1640" yWindow="360" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Micromorts for calculator (2)" sheetId="1" r:id="rId1"/>
@@ -24,33 +24,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="143">
   <si>
-    <t>Event: death from-</t>
-  </si>
-  <si>
-    <t>number of units</t>
-  </si>
-  <si>
-    <t>Unit of exposure</t>
-  </si>
-  <si>
-    <t>micromorts per unit of exposure</t>
-  </si>
-  <si>
     <t>Context</t>
   </si>
   <si>
-    <t>Time period</t>
-  </si>
-  <si>
-    <t>N deaths</t>
-  </si>
-  <si>
-    <t>N population</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>Micromort</t>
   </si>
   <si>
@@ -451,6 +427,30 @@
   </si>
   <si>
     <t>Fisheries</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>micromorts</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>deaths</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>ref</t>
   </si>
 </sst>
 </file>
@@ -993,13 +993,13 @@
   <dimension ref="A1:Y85"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="43.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" style="30" customWidth="1"/>
     <col min="5" max="6" width="17.1640625" customWidth="1"/>
@@ -1009,34 +1009,34 @@
     <col min="11" max="25" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="24">
+    <row r="1" spans="1:25" ht="12">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>138</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>141</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="2" spans="1:25" ht="12">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1091,13 +1091,13 @@
     </row>
     <row r="3" spans="1:25" ht="22">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5">
         <f>(H3*1000000)/(I3)</f>
@@ -1105,7 +1105,7 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G3" s="5">
         <v>2009</v>
@@ -1118,23 +1118,23 @@
         <v>54808000</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="12">
       <c r="A4" s="5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
       <c r="F4" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1143,13 +1143,13 @@
     </row>
     <row r="5" spans="1:25" ht="12">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D5" s="5">
         <f>H5*1000000/I5</f>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G5" s="5">
         <v>2010</v>
@@ -1172,13 +1172,13 @@
     </row>
     <row r="6" spans="1:25" ht="12">
       <c r="A6" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D6" s="5">
         <f>H6*1000000/I6</f>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G6" s="5">
         <v>2010</v>
@@ -1201,13 +1201,13 @@
     </row>
     <row r="7" spans="1:25" ht="12">
       <c r="A7" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D7" s="5">
         <f>H7*1000000/I7</f>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G7" s="5">
         <v>2010</v>
@@ -1230,13 +1230,13 @@
     </row>
     <row r="8" spans="1:25" ht="21" customHeight="1">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D8" s="5">
         <f>H8*1000000/I8</f>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G8" s="5">
         <v>2010</v>
@@ -1256,12 +1256,12 @@
         <v>1000000</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="21" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -1275,13 +1275,13 @@
     </row>
     <row r="10" spans="1:25" ht="12.75" customHeight="1">
       <c r="A10" s="12" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D10" s="30">
         <f t="shared" ref="D10:D17" si="0">H10*1000000/I10</f>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G10" s="5">
         <v>2010</v>
@@ -1301,18 +1301,18 @@
         <v>9500000</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="12.75" customHeight="1">
       <c r="A11" s="14" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D11" s="30">
         <f t="shared" si="0"/>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G11" s="5">
         <v>2011</v>
@@ -1335,13 +1335,13 @@
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1">
       <c r="A12" s="14" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D12" s="30">
         <f t="shared" si="0"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G12" s="5">
         <v>2012</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="13" spans="1:25" ht="12.75" customHeight="1">
       <c r="A13" s="14" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D13" s="30">
         <f t="shared" si="0"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G13" s="5">
         <v>2013</v>
@@ -1393,13 +1393,13 @@
     </row>
     <row r="14" spans="1:25" ht="12.75" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D14" s="30">
         <f t="shared" si="0"/>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G14" s="5">
         <v>2014</v>
@@ -1422,13 +1422,13 @@
     </row>
     <row r="15" spans="1:25" ht="12.75" customHeight="1">
       <c r="A15" s="14" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D15" s="30">
         <f t="shared" si="0"/>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G15" s="5">
         <v>2015</v>
@@ -1451,13 +1451,13 @@
     </row>
     <row r="16" spans="1:25" ht="12.75" customHeight="1">
       <c r="A16" s="14" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D16" s="30">
         <f t="shared" si="0"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G16" s="5">
         <v>2016</v>
@@ -1480,13 +1480,13 @@
     </row>
     <row r="17" spans="1:10" ht="12.75" customHeight="1">
       <c r="A17" s="14" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D17" s="30">
         <f t="shared" si="0"/>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G17" s="5">
         <v>2017</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="18" spans="1:10" ht="27" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -1521,20 +1521,20 @@
     </row>
     <row r="19" spans="1:10" ht="22">
       <c r="A19" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D19" s="5">
         <v>0.3</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G19" s="5">
         <v>2010</v>
@@ -1543,21 +1543,21 @@
         <v>405</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="22">
       <c r="A20" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G20" s="5">
         <v>2010</v>
@@ -1566,25 +1566,25 @@
         <v>62</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="22">
       <c r="A21" s="14" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D21" s="5">
         <v>13.8</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G21" s="5">
         <v>2010</v>
@@ -1593,25 +1593,25 @@
         <v>403</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="12">
       <c r="A22" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B22" s="4">
         <v>1</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D22" s="5">
         <v>3.6</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G22" s="5">
         <v>2010</v>
@@ -1622,20 +1622,20 @@
     </row>
     <row r="23" spans="1:10" ht="12">
       <c r="A23" s="5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D23" s="5">
         <v>3.7</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G23" s="5">
         <v>2010</v>
@@ -1646,18 +1646,18 @@
     </row>
     <row r="24" spans="1:10" ht="12">
       <c r="A24" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G24" s="5">
         <v>2010</v>
@@ -1668,13 +1668,13 @@
     </row>
     <row r="25" spans="1:10" ht="12">
       <c r="A25" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D25" s="5">
         <f>1/75</f>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G25" s="5">
         <v>2010</v>
@@ -1691,23 +1691,23 @@
         <v>0</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="12">
       <c r="A26" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="18"/>
       <c r="F26" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G26" s="5">
         <v>2010</v>
@@ -1715,13 +1715,13 @@
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D27" s="5">
         <f>H27/(I27*10)</f>
@@ -1729,10 +1729,10 @@
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H27" s="5">
         <v>1631</v>
@@ -1741,18 +1741,18 @@
         <v>9714</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D28" s="5">
         <f>H28/(I28*10)</f>
@@ -1760,10 +1760,10 @@
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G28" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H28" s="5">
         <v>166</v>
@@ -1774,13 +1774,13 @@
     </row>
     <row r="29" spans="1:10" ht="12.75" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D29" s="5">
         <f>100/15</f>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1">
@@ -1802,13 +1802,13 @@
     </row>
     <row r="31" spans="1:10" ht="36">
       <c r="A31" s="16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D31" s="5">
         <f t="shared" ref="D31:D40" si="1">D19*I31*0.62/100</f>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G31" s="5">
         <v>2010</v>
@@ -1828,18 +1828,18 @@
         <v>39</v>
       </c>
       <c r="J31" s="21" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="22">
       <c r="A32" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D32" s="5">
         <f>D20*I32*0.62/100</f>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G32" s="5">
         <v>2010</v>
@@ -1856,16 +1856,16 @@
         <v>62</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="22">
       <c r="A33" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D33" s="5">
         <f t="shared" si="1"/>
@@ -1873,7 +1873,7 @@
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G33" s="5">
         <v>2010</v>
@@ -1885,16 +1885,16 @@
         <v>50</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="22">
       <c r="A34" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D34" s="5">
         <f t="shared" si="1"/>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G34" s="5">
         <v>2010</v>
@@ -1914,16 +1914,16 @@
         <v>12.2</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="22">
       <c r="A35" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D35" s="5">
         <f t="shared" si="1"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G35" s="5">
         <v>2010</v>
@@ -1943,16 +1943,16 @@
         <v>4.2</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="22">
       <c r="A36" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D36" s="5">
         <f>D24*I36*0.62/100</f>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G36" s="5">
         <v>2010</v>
@@ -1969,16 +1969,16 @@
         <v>9</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="22">
       <c r="A37" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D37" s="5">
         <f t="shared" si="1"/>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G37" s="5">
         <v>2010</v>
@@ -1998,16 +1998,16 @@
         <v>40</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="12">
       <c r="A38" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D38" s="5">
         <f t="shared" si="1"/>
@@ -2015,7 +2015,7 @@
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G38" s="5">
         <v>2010</v>
@@ -2023,11 +2023,11 @@
     </row>
     <row r="39" spans="1:10" ht="15">
       <c r="A39" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D39" s="5">
         <f t="shared" si="1"/>
@@ -2035,10 +2035,10 @@
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H39" s="5">
         <v>1631</v>
@@ -2050,11 +2050,11 @@
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1">
       <c r="A40" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D40" s="5">
         <f t="shared" si="1"/>
@@ -2067,55 +2067,55 @@
     </row>
     <row r="41" spans="1:10" ht="26" customHeight="1">
       <c r="A41" s="11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:10" ht="24">
       <c r="A42" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D42" s="5">
         <v>10</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="12">
       <c r="A43" s="5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D43" s="5">
         <v>120</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G43" s="5">
         <v>2008</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="12">
       <c r="A44" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -2124,15 +2124,15 @@
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J44" s="8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15">
       <c r="A45" s="23" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2143,39 +2143,39 @@
     </row>
     <row r="46" spans="1:10" ht="33">
       <c r="A46" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D46" s="5">
         <v>47</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H46" s="5">
         <v>60</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15">
       <c r="A47" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D47" s="5">
         <f>(1000000/365)*H47/I47</f>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="E47" s="7"/>
       <c r="F47" s="5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G47" s="5">
         <v>2007</v>
@@ -2195,16 +2195,16 @@
         <v>148000</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15">
       <c r="A48" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D48" s="5">
         <f>(1000000/365)*H48/I48</f>
@@ -2212,7 +2212,7 @@
       </c>
       <c r="E48" s="7"/>
       <c r="F48" s="5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G48" s="5">
         <v>2009</v>
@@ -2224,16 +2224,16 @@
         <v>50700</v>
       </c>
       <c r="J48" s="19" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="12">
       <c r="A49" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D49" s="5">
         <f>(1000000/365)*H49/I49</f>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="E49" s="7"/>
       <c r="F49" s="5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G49" s="5">
         <v>2010</v>
@@ -2253,177 +2253,177 @@
         <v>63500</v>
       </c>
       <c r="J49" s="24" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="24">
       <c r="A50" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D50" s="5">
         <v>27000</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H50" s="5">
         <v>55000</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15">
       <c r="A51" s="23" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B51" s="23"/>
       <c r="C51" s="23"/>
     </row>
     <row r="52" spans="1:10" ht="22">
       <c r="A52" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D52" s="5">
         <v>5</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J52" s="8" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="12">
       <c r="A53" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D53" s="5">
         <v>8</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="12">
       <c r="A54" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D54" s="5">
         <v>3</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="12">
       <c r="A55" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D55" s="5">
         <v>0.7</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="H55" s="5">
         <v>39</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="J55" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="12">
       <c r="A56" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D56" s="5">
         <v>7</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="J56" s="8" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="12">
       <c r="A57" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D57" s="5">
         <v>10</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H57" s="5">
         <v>46</v>
@@ -2432,26 +2432,26 @@
         <v>4700000</v>
       </c>
       <c r="J57" s="8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="15">
       <c r="A58" s="5" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D58" s="5">
         <v>7</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H58" s="5">
         <v>26</v>
@@ -2460,16 +2460,16 @@
         <v>3300000</v>
       </c>
       <c r="J58" s="19" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15">
       <c r="A59" s="5" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
@@ -2481,28 +2481,28 @@
     </row>
     <row r="61" spans="1:10" ht="15">
       <c r="A61" s="23" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="23"/>
     </row>
     <row r="62" spans="1:10" ht="33">
       <c r="A62" s="5" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D62" s="5">
         <v>13410.256410256399</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H62" s="5">
         <v>523</v>
@@ -2511,26 +2511,26 @@
         <v>39</v>
       </c>
       <c r="J62" s="8" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="12">
       <c r="A63" s="5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D63" s="5">
         <v>74.4010088272383</v>
       </c>
       <c r="E63" s="6"/>
       <c r="F63" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H63" s="5">
         <v>59</v>
@@ -2542,21 +2542,21 @@
     </row>
     <row r="64" spans="1:10" ht="12">
       <c r="A64" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D64" s="5">
         <v>53.237410071942399</v>
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H64" s="5">
         <v>22.2</v>
@@ -2568,21 +2568,21 @@
     </row>
     <row r="65" spans="1:10" ht="12">
       <c r="A65" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D65" s="5">
         <v>52.125693160813299</v>
       </c>
       <c r="E65" s="6"/>
       <c r="F65" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H65" s="5">
         <v>28.2</v>
@@ -2594,21 +2594,21 @@
     </row>
     <row r="66" spans="1:10" ht="12">
       <c r="A66" s="5" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D66" s="5">
         <v>0.49382716049383002</v>
       </c>
       <c r="E66" s="6"/>
       <c r="F66" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H66" s="5">
         <v>1.4</v>
@@ -2626,21 +2626,21 @@
     </row>
     <row r="68" spans="1:10" ht="12">
       <c r="A68" s="5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D68" s="5">
         <v>19641.025641025601</v>
       </c>
       <c r="E68" s="6"/>
       <c r="F68" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H68" s="5">
         <v>766</v>
@@ -2652,21 +2652,21 @@
     </row>
     <row r="69" spans="1:10" ht="12">
       <c r="A69" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D69" s="5">
         <v>213.114754098361</v>
       </c>
       <c r="E69" s="6"/>
       <c r="F69" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H69" s="5">
         <v>169</v>
@@ -2678,21 +2678,21 @@
     </row>
     <row r="70" spans="1:10" ht="12">
       <c r="A70" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D70" s="5">
         <v>98.321342925659494</v>
       </c>
       <c r="E70" s="6"/>
       <c r="F70" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H70" s="5">
         <v>41</v>
@@ -2704,21 +2704,21 @@
     </row>
     <row r="71" spans="1:10" ht="12">
       <c r="A71" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D71" s="5">
         <v>90.573012939001799</v>
       </c>
       <c r="E71" s="6"/>
       <c r="F71" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H71" s="5">
         <v>49</v>
@@ -2730,21 +2730,21 @@
     </row>
     <row r="72" spans="1:10" ht="12">
       <c r="A72" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D72" s="5">
         <v>5.5026455026454997</v>
       </c>
       <c r="E72" s="6"/>
       <c r="F72" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H72" s="5">
         <v>15.6</v>
@@ -2756,11 +2756,11 @@
     </row>
     <row r="73" spans="1:10" s="27" customFormat="1" ht="18" customHeight="1">
       <c r="A73" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D73" s="31">
         <f>1000000*H73/I73</f>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="E73" s="26"/>
       <c r="F73" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G73" s="27">
         <v>2012</v>
@@ -2780,12 +2780,12 @@
         <v>335000</v>
       </c>
       <c r="J73" s="17" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="27" customFormat="1" ht="12.75" customHeight="1">
       <c r="A74" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
@@ -2795,7 +2795,7 @@
       </c>
       <c r="E74" s="26"/>
       <c r="F74" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H74" s="31">
         <v>5100</v>
@@ -2807,23 +2807,23 @@
     </row>
     <row r="76" spans="1:10" ht="12.75" customHeight="1">
       <c r="A76" s="22" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B76" s="22"/>
       <c r="C76" s="22"/>
     </row>
     <row r="77" spans="1:10" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C77" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D77" s="30">
         <v>1190</v>
       </c>
       <c r="F77" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G77">
         <v>1911</v>
@@ -2837,33 +2837,33 @@
     </row>
     <row r="78" spans="1:10" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C78" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D78" s="30">
         <v>430</v>
       </c>
       <c r="F78" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G78" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="12.75" customHeight="1">
       <c r="A79" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C79" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D79" s="30">
         <v>6</v>
       </c>
       <c r="F79" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G79">
         <v>2010</v>
@@ -2871,33 +2871,33 @@
     </row>
     <row r="80" spans="1:10" ht="12.75" customHeight="1">
       <c r="A80" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C80" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D80" s="30">
         <v>160</v>
       </c>
       <c r="F80" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="12.75" customHeight="1">
       <c r="A81" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C81" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D81" s="30">
         <v>1020</v>
       </c>
       <c r="F81" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G81" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H81" s="30">
         <v>160</v>
@@ -2905,50 +2905,50 @@
     </row>
     <row r="82" spans="1:10" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C82" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D82" s="30">
         <v>1000</v>
       </c>
       <c r="F82" s="28" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="12.75" customHeight="1">
       <c r="A83" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C83" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D83" s="30">
         <v>1280</v>
       </c>
       <c r="F83" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G83">
         <v>2012</v>
       </c>
       <c r="J83" s="19" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C84" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D84" s="30">
         <v>1100</v>
       </c>
       <c r="F84" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G84">
         <v>2012</v>
@@ -2957,14 +2957,14 @@
     </row>
     <row r="85" spans="1:10" s="22" customFormat="1" ht="12.75" customHeight="1">
       <c r="A85" s="27" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C85" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D85" s="32"/>
       <c r="F85" s="22" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G85" s="22">
         <v>2012</v>

</xml_diff>